<commit_message>
standardized crosswalk between different bug datasest and cleaned up code.
</commit_message>
<xml_diff>
--- a/data/DWR_CageZoop2023_Complete_TEC_1.22.2024.xlsx
+++ b/data/DWR_CageZoop2023_Complete_TEC_1.22.2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/smelt cages/Smelt-cages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2757" documentId="8_{8993E433-6BE3-4E63-A7A0-C5655458F763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D56B7DC0-4B57-4E18-A493-1CC5BA98D8F4}"/>
+  <xr:revisionPtr revIDLastSave="2754" documentId="8_{8993E433-6BE3-4E63-A7A0-C5655458F763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3B2926B-CFE8-41A5-91A0-751B4D5F9179}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="844" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="844" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="8" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Amph Data" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Amph Data'!$A$1:$BL$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Amph Data'!$A$1:$BM$111</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Zoop Data'!$A$1:$N$657</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -2445,14 +2445,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2466,80 +2538,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2591,39 +2624,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6283,19 +6283,19 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="160" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
     </row>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
@@ -6314,35 +6314,35 @@
       <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="135"/>
-      <c r="C3" s="136"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="138"/>
       <c r="E3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="135"/>
-      <c r="G3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="138"/>
       <c r="I3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="135"/>
-      <c r="K3" s="136"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="138"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="135"/>
-      <c r="C4" s="136"/>
+      <c r="B4" s="136"/>
+      <c r="C4" s="138"/>
       <c r="E4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="135"/>
-      <c r="G4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="138"/>
       <c r="I4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="135"/>
-      <c r="K4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="138"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
@@ -6355,31 +6355,31 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
-      <c r="B6" s="135"/>
-      <c r="C6" s="136"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="136"/>
-      <c r="H6" s="147"/>
-      <c r="I6" s="148"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="138"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="138"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="158"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
-      <c r="B7" s="149" t="s">
+      <c r="B7" s="159" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="149"/>
+      <c r="C7" s="159"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="149" t="s">
+      <c r="E7" s="159" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="149"/>
+      <c r="F7" s="159"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="149" t="s">
+      <c r="H7" s="159" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="149"/>
+      <c r="I7" s="159"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
@@ -6412,382 +6412,382 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="137" t="s">
+      <c r="A10" s="161" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="137"/>
-      <c r="C10" s="137"/>
-      <c r="D10" s="137"/>
-      <c r="E10" s="137"/>
-      <c r="G10" s="138" t="s">
+      <c r="B10" s="161"/>
+      <c r="C10" s="161"/>
+      <c r="D10" s="161"/>
+      <c r="E10" s="161"/>
+      <c r="G10" s="162" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="139"/>
-      <c r="I10" s="139"/>
-      <c r="J10" s="139"/>
-      <c r="K10" s="140"/>
+      <c r="H10" s="163"/>
+      <c r="I10" s="163"/>
+      <c r="J10" s="163"/>
+      <c r="K10" s="164"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="141" t="s">
+      <c r="A11" s="154" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="142"/>
-      <c r="C11" s="143"/>
+      <c r="B11" s="155"/>
+      <c r="C11" s="156"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
-      <c r="G11" s="141" t="s">
+      <c r="G11" s="154" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="142"/>
-      <c r="I11" s="143"/>
+      <c r="H11" s="155"/>
+      <c r="I11" s="156"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="144" t="s">
+      <c r="A12" s="147" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="145"/>
-      <c r="C12" s="146"/>
+      <c r="B12" s="134"/>
+      <c r="C12" s="148"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
-      <c r="G12" s="144" t="s">
+      <c r="G12" s="147" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="145"/>
-      <c r="I12" s="146"/>
+      <c r="H12" s="134"/>
+      <c r="I12" s="148"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="144" t="s">
+      <c r="A13" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="145"/>
-      <c r="C13" s="146"/>
+      <c r="B13" s="134"/>
+      <c r="C13" s="148"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
-      <c r="G13" s="144" t="s">
+      <c r="G13" s="147" t="s">
         <v>58</v>
       </c>
-      <c r="H13" s="145"/>
-      <c r="I13" s="146"/>
+      <c r="H13" s="134"/>
+      <c r="I13" s="148"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="147" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="145"/>
-      <c r="C14" s="146"/>
+      <c r="B14" s="134"/>
+      <c r="C14" s="148"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
-      <c r="G14" s="144" t="s">
+      <c r="G14" s="147" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="145"/>
-      <c r="I14" s="146"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="148"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="144" t="s">
+      <c r="A15" s="147" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="145"/>
-      <c r="C15" s="146"/>
+      <c r="B15" s="134"/>
+      <c r="C15" s="148"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
-      <c r="G15" s="144" t="s">
+      <c r="G15" s="147" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="145"/>
-      <c r="I15" s="146"/>
+      <c r="H15" s="134"/>
+      <c r="I15" s="148"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="147" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="145"/>
-      <c r="C16" s="146"/>
+      <c r="B16" s="134"/>
+      <c r="C16" s="148"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
-      <c r="G16" s="144" t="s">
+      <c r="G16" s="147" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="145"/>
-      <c r="I16" s="146"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="148"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="144" t="s">
+      <c r="A17" s="147" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="145"/>
-      <c r="C17" s="146"/>
+      <c r="B17" s="134"/>
+      <c r="C17" s="148"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
-      <c r="G17" s="144" t="s">
+      <c r="G17" s="147" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="145"/>
-      <c r="I17" s="146"/>
+      <c r="H17" s="134"/>
+      <c r="I17" s="148"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="144" t="s">
+      <c r="A18" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="145"/>
-      <c r="C18" s="146"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="148"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
-      <c r="G18" s="144" t="s">
+      <c r="G18" s="147" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="145"/>
-      <c r="I18" s="146"/>
+      <c r="H18" s="134"/>
+      <c r="I18" s="148"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="144" t="s">
+      <c r="A19" s="147" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="145"/>
-      <c r="C19" s="146"/>
+      <c r="B19" s="134"/>
+      <c r="C19" s="148"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
-      <c r="G19" s="144" t="s">
+      <c r="G19" s="147" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="145"/>
-      <c r="I19" s="146"/>
+      <c r="H19" s="134"/>
+      <c r="I19" s="148"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="144" t="s">
+      <c r="A20" s="147" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="145"/>
-      <c r="C20" s="146"/>
+      <c r="B20" s="134"/>
+      <c r="C20" s="148"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
-      <c r="G20" s="144" t="s">
+      <c r="G20" s="147" t="s">
         <v>72</v>
       </c>
-      <c r="H20" s="145"/>
-      <c r="I20" s="146"/>
+      <c r="H20" s="134"/>
+      <c r="I20" s="148"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="144" t="s">
+      <c r="A21" s="147" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="145"/>
-      <c r="C21" s="146"/>
+      <c r="B21" s="134"/>
+      <c r="C21" s="148"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
-      <c r="G21" s="144" t="s">
+      <c r="G21" s="147" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="145"/>
-      <c r="I21" s="146"/>
+      <c r="H21" s="134"/>
+      <c r="I21" s="148"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="144" t="s">
+      <c r="A22" s="147" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="145"/>
-      <c r="C22" s="146"/>
+      <c r="B22" s="134"/>
+      <c r="C22" s="148"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="G22" s="144" t="s">
+      <c r="G22" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="145"/>
-      <c r="I22" s="146"/>
+      <c r="H22" s="134"/>
+      <c r="I22" s="148"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="144" t="s">
+      <c r="A23" s="147" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="145"/>
-      <c r="C23" s="146"/>
+      <c r="B23" s="134"/>
+      <c r="C23" s="148"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="G23" s="144" t="s">
+      <c r="G23" s="147" t="s">
         <v>78</v>
       </c>
-      <c r="H23" s="145"/>
-      <c r="I23" s="146"/>
+      <c r="H23" s="134"/>
+      <c r="I23" s="148"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="144" t="s">
+      <c r="A24" s="147" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="145"/>
-      <c r="C24" s="146"/>
+      <c r="B24" s="134"/>
+      <c r="C24" s="148"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
-      <c r="G24" s="144" t="s">
+      <c r="G24" s="147" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="145"/>
-      <c r="I24" s="146"/>
+      <c r="H24" s="134"/>
+      <c r="I24" s="148"/>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="144" t="s">
+      <c r="A25" s="147" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="145"/>
-      <c r="C25" s="146"/>
+      <c r="B25" s="134"/>
+      <c r="C25" s="148"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
-      <c r="G25" s="144" t="s">
+      <c r="G25" s="147" t="s">
         <v>82</v>
       </c>
-      <c r="H25" s="145"/>
-      <c r="I25" s="146"/>
+      <c r="H25" s="134"/>
+      <c r="I25" s="148"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="144" t="s">
+      <c r="A26" s="147" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="145"/>
-      <c r="C26" s="146"/>
+      <c r="B26" s="134"/>
+      <c r="C26" s="148"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
-      <c r="G26" s="144" t="s">
+      <c r="G26" s="147" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="145"/>
-      <c r="I26" s="146"/>
+      <c r="H26" s="134"/>
+      <c r="I26" s="148"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="144" t="s">
+      <c r="A27" s="147" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="145"/>
-      <c r="C27" s="146"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="148"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
-      <c r="G27" s="144" t="s">
+      <c r="G27" s="147" t="s">
         <v>86</v>
       </c>
-      <c r="H27" s="145"/>
-      <c r="I27" s="146"/>
+      <c r="H27" s="134"/>
+      <c r="I27" s="148"/>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="144" t="s">
+      <c r="A28" s="147" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="145"/>
-      <c r="C28" s="146"/>
+      <c r="B28" s="134"/>
+      <c r="C28" s="148"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
-      <c r="G28" s="144" t="s">
+      <c r="G28" s="147" t="s">
         <v>88</v>
       </c>
-      <c r="H28" s="145"/>
-      <c r="I28" s="146"/>
+      <c r="H28" s="134"/>
+      <c r="I28" s="148"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="144" t="s">
+      <c r="A29" s="147" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="145"/>
-      <c r="C29" s="146"/>
+      <c r="B29" s="134"/>
+      <c r="C29" s="148"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
-      <c r="G29" s="144" t="s">
+      <c r="G29" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="H29" s="145"/>
-      <c r="I29" s="146"/>
+      <c r="H29" s="134"/>
+      <c r="I29" s="148"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="144" t="s">
+      <c r="A30" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="145"/>
-      <c r="C30" s="146"/>
+      <c r="B30" s="134"/>
+      <c r="C30" s="148"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
-      <c r="G30" s="144" t="s">
+      <c r="G30" s="147" t="s">
         <v>92</v>
       </c>
-      <c r="H30" s="145"/>
-      <c r="I30" s="146"/>
+      <c r="H30" s="134"/>
+      <c r="I30" s="148"/>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="144" t="s">
+      <c r="A31" s="147" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="145"/>
-      <c r="C31" s="146"/>
+      <c r="B31" s="134"/>
+      <c r="C31" s="148"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
-      <c r="G31" s="144" t="s">
+      <c r="G31" s="147" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="145"/>
-      <c r="I31" s="146"/>
+      <c r="H31" s="134"/>
+      <c r="I31" s="148"/>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="144"/>
-      <c r="B32" s="145"/>
-      <c r="C32" s="146"/>
+      <c r="A32" s="147"/>
+      <c r="B32" s="134"/>
+      <c r="C32" s="148"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
-      <c r="G32" s="144" t="s">
+      <c r="G32" s="147" t="s">
         <v>95</v>
       </c>
-      <c r="H32" s="145"/>
-      <c r="I32" s="146"/>
+      <c r="H32" s="134"/>
+      <c r="I32" s="148"/>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="144"/>
-      <c r="B33" s="145"/>
-      <c r="C33" s="146"/>
+      <c r="A33" s="147"/>
+      <c r="B33" s="134"/>
+      <c r="C33" s="148"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
-      <c r="G33" s="144" t="s">
+      <c r="G33" s="147" t="s">
         <v>96</v>
       </c>
-      <c r="H33" s="145"/>
-      <c r="I33" s="146"/>
+      <c r="H33" s="134"/>
+      <c r="I33" s="148"/>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
     </row>
@@ -6795,110 +6795,110 @@
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
-      <c r="G34" s="144" t="s">
+      <c r="G34" s="147" t="s">
         <v>97</v>
       </c>
-      <c r="H34" s="145"/>
-      <c r="I34" s="146"/>
+      <c r="H34" s="134"/>
+      <c r="I34" s="148"/>
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" s="150" t="s">
+      <c r="A35" s="149" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="150"/>
-      <c r="C35" s="150"/>
-      <c r="D35" s="150"/>
-      <c r="E35" s="150"/>
-      <c r="G35" s="144" t="s">
+      <c r="B35" s="149"/>
+      <c r="C35" s="149"/>
+      <c r="D35" s="149"/>
+      <c r="E35" s="149"/>
+      <c r="G35" s="147" t="s">
         <v>99</v>
       </c>
-      <c r="H35" s="145"/>
-      <c r="I35" s="146"/>
+      <c r="H35" s="134"/>
+      <c r="I35" s="148"/>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="151" t="s">
+      <c r="A36" s="150" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="151"/>
-      <c r="C36" s="151"/>
+      <c r="B36" s="150"/>
+      <c r="C36" s="150"/>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
-      <c r="G36" s="144" t="s">
+      <c r="G36" s="147" t="s">
         <v>101</v>
       </c>
-      <c r="H36" s="145"/>
-      <c r="I36" s="146"/>
+      <c r="H36" s="134"/>
+      <c r="I36" s="148"/>
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="152" t="s">
+      <c r="A37" s="135" t="s">
         <v>102</v>
       </c>
-      <c r="B37" s="152"/>
-      <c r="C37" s="152"/>
+      <c r="B37" s="135"/>
+      <c r="C37" s="135"/>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
-      <c r="G37" s="144" t="s">
+      <c r="G37" s="147" t="s">
         <v>103</v>
       </c>
-      <c r="H37" s="145"/>
-      <c r="I37" s="146"/>
+      <c r="H37" s="134"/>
+      <c r="I37" s="148"/>
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" s="152" t="s">
+      <c r="A38" s="135" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="152"/>
-      <c r="C38" s="152"/>
+      <c r="B38" s="135"/>
+      <c r="C38" s="135"/>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
-      <c r="G38" s="144"/>
-      <c r="H38" s="145"/>
-      <c r="I38" s="146"/>
+      <c r="G38" s="147"/>
+      <c r="H38" s="134"/>
+      <c r="I38" s="148"/>
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="152" t="s">
+      <c r="A39" s="135" t="s">
         <v>105</v>
       </c>
-      <c r="B39" s="152"/>
-      <c r="C39" s="152"/>
+      <c r="B39" s="135"/>
+      <c r="C39" s="135"/>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
-      <c r="G39" s="144"/>
-      <c r="H39" s="145"/>
-      <c r="I39" s="146"/>
+      <c r="G39" s="147"/>
+      <c r="H39" s="134"/>
+      <c r="I39" s="148"/>
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="152" t="s">
+      <c r="A40" s="135" t="s">
         <v>106</v>
       </c>
-      <c r="B40" s="152"/>
-      <c r="C40" s="152"/>
+      <c r="B40" s="135"/>
+      <c r="C40" s="135"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
-      <c r="G40" s="144"/>
-      <c r="H40" s="145"/>
-      <c r="I40" s="146"/>
+      <c r="G40" s="147"/>
+      <c r="H40" s="134"/>
+      <c r="I40" s="148"/>
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="152" t="s">
+      <c r="A41" s="135" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="152"/>
-      <c r="C41" s="152"/>
+      <c r="B41" s="135"/>
+      <c r="C41" s="135"/>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
       <c r="G41" s="14"/>
@@ -6906,334 +6906,334 @@
       <c r="I41" s="14"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="152" t="s">
+      <c r="A42" s="135" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="152"/>
-      <c r="C42" s="152"/>
+      <c r="B42" s="135"/>
+      <c r="C42" s="135"/>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
-      <c r="G42" s="153" t="s">
+      <c r="G42" s="141" t="s">
         <v>109</v>
       </c>
-      <c r="H42" s="154"/>
-      <c r="I42" s="154"/>
-      <c r="J42" s="154"/>
-      <c r="K42" s="155"/>
+      <c r="H42" s="142"/>
+      <c r="I42" s="142"/>
+      <c r="J42" s="142"/>
+      <c r="K42" s="143"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="152" t="s">
+      <c r="A43" s="135" t="s">
         <v>110</v>
       </c>
-      <c r="B43" s="152"/>
-      <c r="C43" s="152"/>
+      <c r="B43" s="135"/>
+      <c r="C43" s="135"/>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
-      <c r="G43" s="156" t="s">
+      <c r="G43" s="152" t="s">
         <v>111</v>
       </c>
-      <c r="H43" s="157"/>
-      <c r="I43" s="158"/>
+      <c r="H43" s="139"/>
+      <c r="I43" s="153"/>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="152" t="s">
+      <c r="A44" s="135" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="152"/>
-      <c r="C44" s="152"/>
+      <c r="B44" s="135"/>
+      <c r="C44" s="135"/>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
-      <c r="G44" s="144" t="s">
+      <c r="G44" s="147" t="s">
         <v>113</v>
       </c>
-      <c r="H44" s="145"/>
-      <c r="I44" s="146"/>
+      <c r="H44" s="134"/>
+      <c r="I44" s="148"/>
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="152" t="s">
+      <c r="A45" s="135" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="152"/>
-      <c r="C45" s="152"/>
+      <c r="B45" s="135"/>
+      <c r="C45" s="135"/>
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
-      <c r="G45" s="144" t="s">
+      <c r="G45" s="147" t="s">
         <v>115</v>
       </c>
-      <c r="H45" s="145"/>
-      <c r="I45" s="146"/>
+      <c r="H45" s="134"/>
+      <c r="I45" s="148"/>
       <c r="J45" s="13"/>
       <c r="K45" s="13"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" s="152" t="s">
+      <c r="A46" s="135" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="152"/>
-      <c r="C46" s="152"/>
+      <c r="B46" s="135"/>
+      <c r="C46" s="135"/>
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
-      <c r="G46" s="144" t="s">
+      <c r="G46" s="147" t="s">
         <v>117</v>
       </c>
-      <c r="H46" s="145"/>
-      <c r="I46" s="146"/>
+      <c r="H46" s="134"/>
+      <c r="I46" s="148"/>
       <c r="J46" s="13"/>
       <c r="K46" s="13"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" s="152" t="s">
+      <c r="A47" s="135" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="152"/>
-      <c r="C47" s="152"/>
+      <c r="B47" s="135"/>
+      <c r="C47" s="135"/>
       <c r="D47" s="13"/>
       <c r="E47" s="13"/>
-      <c r="G47" s="144" t="s">
+      <c r="G47" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="H47" s="145"/>
-      <c r="I47" s="146"/>
+      <c r="H47" s="134"/>
+      <c r="I47" s="148"/>
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" s="152" t="s">
+      <c r="A48" s="135" t="s">
         <v>120</v>
       </c>
-      <c r="B48" s="152"/>
-      <c r="C48" s="152"/>
+      <c r="B48" s="135"/>
+      <c r="C48" s="135"/>
       <c r="D48" s="13"/>
       <c r="E48" s="13"/>
-      <c r="G48" s="144" t="s">
+      <c r="G48" s="147" t="s">
         <v>121</v>
       </c>
-      <c r="H48" s="145"/>
-      <c r="I48" s="146"/>
+      <c r="H48" s="134"/>
+      <c r="I48" s="148"/>
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="152" t="s">
+      <c r="A49" s="135" t="s">
         <v>122</v>
       </c>
-      <c r="B49" s="152"/>
-      <c r="C49" s="152"/>
+      <c r="B49" s="135"/>
+      <c r="C49" s="135"/>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
-      <c r="G49" s="144" t="s">
+      <c r="G49" s="147" t="s">
         <v>123</v>
       </c>
-      <c r="H49" s="145"/>
-      <c r="I49" s="146"/>
+      <c r="H49" s="134"/>
+      <c r="I49" s="148"/>
       <c r="J49" s="13"/>
       <c r="K49" s="13"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A50" s="152" t="s">
+      <c r="A50" s="135" t="s">
         <v>124</v>
       </c>
-      <c r="B50" s="152"/>
-      <c r="C50" s="152"/>
+      <c r="B50" s="135"/>
+      <c r="C50" s="135"/>
       <c r="D50" s="13"/>
       <c r="E50" s="13"/>
-      <c r="G50" s="144" t="s">
+      <c r="G50" s="147" t="s">
         <v>125</v>
       </c>
-      <c r="H50" s="145"/>
-      <c r="I50" s="146"/>
+      <c r="H50" s="134"/>
+      <c r="I50" s="148"/>
       <c r="J50" s="13"/>
       <c r="K50" s="13"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A51" s="152" t="s">
+      <c r="A51" s="135" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="152"/>
-      <c r="C51" s="152"/>
+      <c r="B51" s="135"/>
+      <c r="C51" s="135"/>
       <c r="D51" s="13"/>
       <c r="E51" s="13"/>
-      <c r="G51" s="144" t="s">
+      <c r="G51" s="147" t="s">
         <v>127</v>
       </c>
-      <c r="H51" s="145"/>
-      <c r="I51" s="146"/>
+      <c r="H51" s="134"/>
+      <c r="I51" s="148"/>
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52" s="152" t="s">
+      <c r="A52" s="135" t="s">
         <v>128</v>
       </c>
-      <c r="B52" s="152"/>
-      <c r="C52" s="152"/>
+      <c r="B52" s="135"/>
+      <c r="C52" s="135"/>
       <c r="D52" s="13"/>
       <c r="E52" s="13"/>
-      <c r="G52" s="144" t="s">
+      <c r="G52" s="147" t="s">
         <v>129</v>
       </c>
-      <c r="H52" s="145"/>
-      <c r="I52" s="146"/>
+      <c r="H52" s="134"/>
+      <c r="I52" s="148"/>
       <c r="J52" s="13"/>
       <c r="K52" s="13"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A53" s="152" t="s">
+      <c r="A53" s="135" t="s">
         <v>130</v>
       </c>
-      <c r="B53" s="152"/>
-      <c r="C53" s="152"/>
+      <c r="B53" s="135"/>
+      <c r="C53" s="135"/>
       <c r="D53" s="13"/>
       <c r="E53" s="13"/>
-      <c r="G53" s="144" t="s">
+      <c r="G53" s="147" t="s">
         <v>131</v>
       </c>
-      <c r="H53" s="145"/>
-      <c r="I53" s="146"/>
+      <c r="H53" s="134"/>
+      <c r="I53" s="148"/>
       <c r="J53" s="13"/>
       <c r="K53" s="13"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A54" s="152" t="s">
+      <c r="A54" s="135" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="152"/>
-      <c r="C54" s="152"/>
+      <c r="B54" s="135"/>
+      <c r="C54" s="135"/>
       <c r="D54" s="13"/>
       <c r="E54" s="13"/>
-      <c r="G54" s="144" t="s">
+      <c r="G54" s="147" t="s">
         <v>133</v>
       </c>
-      <c r="H54" s="145"/>
-      <c r="I54" s="146"/>
+      <c r="H54" s="134"/>
+      <c r="I54" s="148"/>
       <c r="J54" s="13"/>
       <c r="K54" s="13"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A55" s="152" t="s">
+      <c r="A55" s="135" t="s">
         <v>134</v>
       </c>
-      <c r="B55" s="152"/>
-      <c r="C55" s="152"/>
+      <c r="B55" s="135"/>
+      <c r="C55" s="135"/>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
-      <c r="G55" s="144" t="s">
+      <c r="G55" s="147" t="s">
         <v>135</v>
       </c>
-      <c r="H55" s="145"/>
-      <c r="I55" s="146"/>
+      <c r="H55" s="134"/>
+      <c r="I55" s="148"/>
       <c r="J55" s="13"/>
       <c r="K55" s="13"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A56" s="152" t="s">
+      <c r="A56" s="135" t="s">
         <v>136</v>
       </c>
-      <c r="B56" s="152"/>
-      <c r="C56" s="152"/>
+      <c r="B56" s="135"/>
+      <c r="C56" s="135"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
-      <c r="G56" s="144" t="s">
+      <c r="G56" s="147" t="s">
         <v>137</v>
       </c>
-      <c r="H56" s="145"/>
-      <c r="I56" s="146"/>
+      <c r="H56" s="134"/>
+      <c r="I56" s="148"/>
       <c r="J56" s="13"/>
       <c r="K56" s="13"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A57" s="152" t="s">
+      <c r="A57" s="135" t="s">
         <v>138</v>
       </c>
-      <c r="B57" s="152"/>
-      <c r="C57" s="152"/>
+      <c r="B57" s="135"/>
+      <c r="C57" s="135"/>
       <c r="D57" s="13"/>
       <c r="E57" s="13"/>
-      <c r="G57" s="144" t="s">
+      <c r="G57" s="147" t="s">
         <v>139</v>
       </c>
-      <c r="H57" s="145"/>
-      <c r="I57" s="146"/>
+      <c r="H57" s="134"/>
+      <c r="I57" s="148"/>
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A58" s="152" t="s">
+      <c r="A58" s="135" t="s">
         <v>140</v>
       </c>
-      <c r="B58" s="152"/>
-      <c r="C58" s="152"/>
+      <c r="B58" s="135"/>
+      <c r="C58" s="135"/>
       <c r="D58" s="13"/>
       <c r="E58" s="13"/>
-      <c r="G58" s="144" t="s">
+      <c r="G58" s="147" t="s">
         <v>141</v>
       </c>
-      <c r="H58" s="145"/>
-      <c r="I58" s="146"/>
+      <c r="H58" s="134"/>
+      <c r="I58" s="148"/>
       <c r="J58" s="13"/>
       <c r="K58" s="13"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A59" s="152" t="s">
+      <c r="A59" s="135" t="s">
         <v>142</v>
       </c>
-      <c r="B59" s="152"/>
-      <c r="C59" s="152"/>
+      <c r="B59" s="135"/>
+      <c r="C59" s="135"/>
       <c r="D59" s="13"/>
       <c r="E59" s="13"/>
-      <c r="G59" s="144" t="s">
+      <c r="G59" s="147" t="s">
         <v>143</v>
       </c>
-      <c r="H59" s="145"/>
-      <c r="I59" s="146"/>
+      <c r="H59" s="134"/>
+      <c r="I59" s="148"/>
       <c r="J59" s="13"/>
       <c r="K59" s="13"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A60" s="152" t="s">
+      <c r="A60" s="135" t="s">
         <v>144</v>
       </c>
-      <c r="B60" s="152"/>
-      <c r="C60" s="152"/>
+      <c r="B60" s="135"/>
+      <c r="C60" s="135"/>
       <c r="D60" s="13"/>
       <c r="E60" s="13"/>
-      <c r="G60" s="144" t="s">
+      <c r="G60" s="147" t="s">
         <v>145</v>
       </c>
-      <c r="H60" s="145"/>
-      <c r="I60" s="146"/>
+      <c r="H60" s="134"/>
+      <c r="I60" s="148"/>
       <c r="J60" s="13"/>
       <c r="K60" s="13"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A61" s="159"/>
-      <c r="B61" s="159"/>
-      <c r="C61" s="159"/>
+      <c r="A61" s="151"/>
+      <c r="B61" s="151"/>
+      <c r="C61" s="151"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
-      <c r="G61" s="144" t="s">
+      <c r="G61" s="147" t="s">
         <v>146</v>
       </c>
-      <c r="H61" s="145"/>
-      <c r="I61" s="146"/>
+      <c r="H61" s="134"/>
+      <c r="I61" s="148"/>
       <c r="J61" s="13"/>
       <c r="K61" s="13"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A62" s="159"/>
-      <c r="B62" s="159"/>
-      <c r="C62" s="159"/>
+      <c r="A62" s="151"/>
+      <c r="B62" s="151"/>
+      <c r="C62" s="151"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
-      <c r="G62" s="144" t="s">
+      <c r="G62" s="147" t="s">
         <v>147</v>
       </c>
-      <c r="H62" s="145"/>
-      <c r="I62" s="146"/>
+      <c r="H62" s="134"/>
+      <c r="I62" s="148"/>
       <c r="J62" s="13"/>
       <c r="K62" s="13"/>
     </row>
@@ -7241,144 +7241,144 @@
       <c r="A63" s="15"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
-      <c r="G63" s="144" t="s">
+      <c r="G63" s="147" t="s">
         <v>148</v>
       </c>
-      <c r="H63" s="145"/>
-      <c r="I63" s="146"/>
+      <c r="H63" s="134"/>
+      <c r="I63" s="148"/>
       <c r="J63" s="13"/>
       <c r="K63" s="13"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A64" s="150" t="s">
+      <c r="A64" s="149" t="s">
         <v>149</v>
       </c>
-      <c r="B64" s="150"/>
-      <c r="C64" s="150"/>
-      <c r="D64" s="150"/>
-      <c r="E64" s="150"/>
-      <c r="G64" s="144" t="s">
+      <c r="B64" s="149"/>
+      <c r="C64" s="149"/>
+      <c r="D64" s="149"/>
+      <c r="E64" s="149"/>
+      <c r="G64" s="147" t="s">
         <v>150</v>
       </c>
-      <c r="H64" s="145"/>
-      <c r="I64" s="146"/>
+      <c r="H64" s="134"/>
+      <c r="I64" s="148"/>
       <c r="J64" s="13"/>
       <c r="K64" s="13"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A65" s="151" t="s">
+      <c r="A65" s="150" t="s">
         <v>151</v>
       </c>
-      <c r="B65" s="151"/>
-      <c r="C65" s="151"/>
+      <c r="B65" s="150"/>
+      <c r="C65" s="150"/>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
-      <c r="G65" s="144" t="s">
+      <c r="G65" s="147" t="s">
         <v>152</v>
       </c>
-      <c r="H65" s="145"/>
-      <c r="I65" s="146"/>
+      <c r="H65" s="134"/>
+      <c r="I65" s="148"/>
       <c r="J65" s="13"/>
       <c r="K65" s="13"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A66" s="152" t="s">
+      <c r="A66" s="135" t="s">
         <v>153</v>
       </c>
-      <c r="B66" s="152"/>
-      <c r="C66" s="152"/>
+      <c r="B66" s="135"/>
+      <c r="C66" s="135"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
-      <c r="G66" s="144" t="s">
+      <c r="G66" s="147" t="s">
         <v>154</v>
       </c>
-      <c r="H66" s="145"/>
-      <c r="I66" s="146"/>
+      <c r="H66" s="134"/>
+      <c r="I66" s="148"/>
       <c r="J66" s="13"/>
       <c r="K66" s="13"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A67" s="152" t="s">
+      <c r="A67" s="135" t="s">
         <v>155</v>
       </c>
-      <c r="B67" s="152"/>
-      <c r="C67" s="152"/>
+      <c r="B67" s="135"/>
+      <c r="C67" s="135"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
-      <c r="G67" s="144" t="s">
+      <c r="G67" s="147" t="s">
         <v>156</v>
       </c>
-      <c r="H67" s="145"/>
-      <c r="I67" s="146"/>
+      <c r="H67" s="134"/>
+      <c r="I67" s="148"/>
       <c r="J67" s="13"/>
       <c r="K67" s="13"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A68" s="152" t="s">
+      <c r="A68" s="135" t="s">
         <v>157</v>
       </c>
-      <c r="B68" s="152"/>
-      <c r="C68" s="152"/>
+      <c r="B68" s="135"/>
+      <c r="C68" s="135"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
-      <c r="G68" s="144" t="s">
+      <c r="G68" s="147" t="s">
         <v>158</v>
       </c>
-      <c r="H68" s="145"/>
-      <c r="I68" s="146"/>
+      <c r="H68" s="134"/>
+      <c r="I68" s="148"/>
       <c r="J68" s="13"/>
       <c r="K68" s="13"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A69" s="152" t="s">
+      <c r="A69" s="135" t="s">
         <v>159</v>
       </c>
-      <c r="B69" s="152"/>
-      <c r="C69" s="152"/>
+      <c r="B69" s="135"/>
+      <c r="C69" s="135"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
-      <c r="G69" s="144" t="s">
+      <c r="G69" s="147" t="s">
         <v>160</v>
       </c>
-      <c r="H69" s="145"/>
-      <c r="I69" s="146"/>
+      <c r="H69" s="134"/>
+      <c r="I69" s="148"/>
       <c r="J69" s="13"/>
       <c r="K69" s="13"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A70" s="152" t="s">
+      <c r="A70" s="135" t="s">
         <v>161</v>
       </c>
-      <c r="B70" s="152"/>
-      <c r="C70" s="152"/>
+      <c r="B70" s="135"/>
+      <c r="C70" s="135"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
-      <c r="G70" s="135"/>
-      <c r="H70" s="164"/>
-      <c r="I70" s="136"/>
+      <c r="G70" s="136"/>
+      <c r="H70" s="137"/>
+      <c r="I70" s="138"/>
       <c r="J70" s="13"/>
       <c r="K70" s="13"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A71" s="152" t="s">
+      <c r="A71" s="135" t="s">
         <v>162</v>
       </c>
-      <c r="B71" s="152"/>
-      <c r="C71" s="152"/>
+      <c r="B71" s="135"/>
+      <c r="C71" s="135"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
-      <c r="G71" s="135"/>
-      <c r="H71" s="164"/>
-      <c r="I71" s="136"/>
+      <c r="G71" s="136"/>
+      <c r="H71" s="137"/>
+      <c r="I71" s="138"/>
       <c r="J71" s="13"/>
       <c r="K71" s="13"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A72" s="152" t="s">
+      <c r="A72" s="135" t="s">
         <v>163</v>
       </c>
-      <c r="B72" s="152"/>
-      <c r="C72" s="152"/>
+      <c r="B72" s="135"/>
+      <c r="C72" s="135"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
       <c r="G72" s="15"/>
@@ -7386,215 +7386,215 @@
       <c r="I72" s="15"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A73" s="152" t="s">
+      <c r="A73" s="135" t="s">
         <v>164</v>
       </c>
-      <c r="B73" s="152"/>
-      <c r="C73" s="152"/>
+      <c r="B73" s="135"/>
+      <c r="C73" s="135"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
-      <c r="G73" s="153" t="s">
+      <c r="G73" s="141" t="s">
         <v>165</v>
       </c>
-      <c r="H73" s="154"/>
-      <c r="I73" s="155"/>
+      <c r="H73" s="142"/>
+      <c r="I73" s="143"/>
       <c r="J73" s="13"/>
       <c r="K73" s="13"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A74" s="152" t="s">
+      <c r="A74" s="135" t="s">
         <v>166</v>
       </c>
-      <c r="B74" s="152"/>
-      <c r="C74" s="152"/>
+      <c r="B74" s="135"/>
+      <c r="C74" s="135"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
-      <c r="G74" s="160"/>
-      <c r="H74" s="160"/>
-      <c r="I74" s="160"/>
+      <c r="G74" s="140"/>
+      <c r="H74" s="140"/>
+      <c r="I74" s="140"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A75" s="152" t="s">
+      <c r="A75" s="135" t="s">
         <v>167</v>
       </c>
-      <c r="B75" s="152"/>
-      <c r="C75" s="152"/>
+      <c r="B75" s="135"/>
+      <c r="C75" s="135"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
-      <c r="G75" s="153" t="s">
+      <c r="G75" s="141" t="s">
         <v>168</v>
       </c>
-      <c r="H75" s="154"/>
-      <c r="I75" s="154"/>
-      <c r="J75" s="154"/>
-      <c r="K75" s="155"/>
+      <c r="H75" s="142"/>
+      <c r="I75" s="142"/>
+      <c r="J75" s="142"/>
+      <c r="K75" s="143"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A76" s="152" t="s">
+      <c r="A76" s="135" t="s">
         <v>169</v>
       </c>
-      <c r="B76" s="152"/>
-      <c r="C76" s="152"/>
+      <c r="B76" s="135"/>
+      <c r="C76" s="135"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
-      <c r="G76" s="161"/>
-      <c r="H76" s="162"/>
-      <c r="I76" s="163"/>
+      <c r="G76" s="144"/>
+      <c r="H76" s="145"/>
+      <c r="I76" s="146"/>
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A77" s="152" t="s">
+      <c r="A77" s="135" t="s">
         <v>170</v>
       </c>
-      <c r="B77" s="152"/>
-      <c r="C77" s="152"/>
+      <c r="B77" s="135"/>
+      <c r="C77" s="135"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
-      <c r="G77" s="135"/>
-      <c r="H77" s="164"/>
-      <c r="I77" s="136"/>
+      <c r="G77" s="136"/>
+      <c r="H77" s="137"/>
+      <c r="I77" s="138"/>
       <c r="J77" s="13"/>
       <c r="K77" s="13"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A78" s="152" t="s">
+      <c r="A78" s="135" t="s">
         <v>171</v>
       </c>
-      <c r="B78" s="152"/>
-      <c r="C78" s="152"/>
+      <c r="B78" s="135"/>
+      <c r="C78" s="135"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
-      <c r="G78" s="135"/>
-      <c r="H78" s="164"/>
-      <c r="I78" s="136"/>
+      <c r="G78" s="136"/>
+      <c r="H78" s="137"/>
+      <c r="I78" s="138"/>
       <c r="J78" s="13"/>
       <c r="K78" s="13"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A79" s="152" t="s">
+      <c r="A79" s="135" t="s">
         <v>172</v>
       </c>
-      <c r="B79" s="152"/>
-      <c r="C79" s="152"/>
+      <c r="B79" s="135"/>
+      <c r="C79" s="135"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
-      <c r="G79" s="135"/>
-      <c r="H79" s="164"/>
-      <c r="I79" s="136"/>
+      <c r="G79" s="136"/>
+      <c r="H79" s="137"/>
+      <c r="I79" s="138"/>
       <c r="J79" s="13"/>
       <c r="K79" s="13"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A80" s="152" t="s">
+      <c r="A80" s="135" t="s">
         <v>173</v>
       </c>
-      <c r="B80" s="152"/>
-      <c r="C80" s="152"/>
+      <c r="B80" s="135"/>
+      <c r="C80" s="135"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
-      <c r="G80" s="135"/>
-      <c r="H80" s="164"/>
-      <c r="I80" s="136"/>
+      <c r="G80" s="136"/>
+      <c r="H80" s="137"/>
+      <c r="I80" s="138"/>
       <c r="J80" s="13"/>
       <c r="K80" s="13"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A81" s="152" t="s">
+      <c r="A81" s="135" t="s">
         <v>174</v>
       </c>
-      <c r="B81" s="152"/>
-      <c r="C81" s="152"/>
+      <c r="B81" s="135"/>
+      <c r="C81" s="135"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
-      <c r="G81" s="135"/>
-      <c r="H81" s="164"/>
-      <c r="I81" s="136"/>
+      <c r="G81" s="136"/>
+      <c r="H81" s="137"/>
+      <c r="I81" s="138"/>
       <c r="J81" s="13"/>
       <c r="K81" s="13"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A82" s="152" t="s">
+      <c r="A82" s="135" t="s">
         <v>175</v>
       </c>
-      <c r="B82" s="152"/>
-      <c r="C82" s="152"/>
+      <c r="B82" s="135"/>
+      <c r="C82" s="135"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
-      <c r="G82" s="135"/>
-      <c r="H82" s="164"/>
-      <c r="I82" s="136"/>
+      <c r="G82" s="136"/>
+      <c r="H82" s="137"/>
+      <c r="I82" s="138"/>
       <c r="J82" s="13"/>
       <c r="K82" s="13"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A83" s="152" t="s">
+      <c r="A83" s="135" t="s">
         <v>176</v>
       </c>
-      <c r="B83" s="152"/>
-      <c r="C83" s="152"/>
+      <c r="B83" s="135"/>
+      <c r="C83" s="135"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
-      <c r="G83" s="135"/>
-      <c r="H83" s="164"/>
-      <c r="I83" s="136"/>
+      <c r="G83" s="136"/>
+      <c r="H83" s="137"/>
+      <c r="I83" s="138"/>
       <c r="J83" s="13"/>
       <c r="K83" s="13"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A84" s="152" t="s">
+      <c r="A84" s="135" t="s">
         <v>177</v>
       </c>
-      <c r="B84" s="152"/>
-      <c r="C84" s="152"/>
+      <c r="B84" s="135"/>
+      <c r="C84" s="135"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
-      <c r="G84" s="135"/>
-      <c r="H84" s="164"/>
-      <c r="I84" s="136"/>
+      <c r="G84" s="136"/>
+      <c r="H84" s="137"/>
+      <c r="I84" s="138"/>
       <c r="J84" s="13"/>
       <c r="K84" s="13"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A85" s="152" t="s">
+      <c r="A85" s="135" t="s">
         <v>178</v>
       </c>
-      <c r="B85" s="152"/>
-      <c r="C85" s="152"/>
+      <c r="B85" s="135"/>
+      <c r="C85" s="135"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
-      <c r="G85" s="135"/>
-      <c r="H85" s="164"/>
-      <c r="I85" s="136"/>
+      <c r="G85" s="136"/>
+      <c r="H85" s="137"/>
+      <c r="I85" s="138"/>
       <c r="J85" s="13"/>
       <c r="K85" s="13"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A86" s="152" t="s">
+      <c r="A86" s="135" t="s">
         <v>179</v>
       </c>
-      <c r="B86" s="152"/>
-      <c r="C86" s="152"/>
+      <c r="B86" s="135"/>
+      <c r="C86" s="135"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
-      <c r="G86" s="135"/>
-      <c r="H86" s="164"/>
-      <c r="I86" s="136"/>
+      <c r="G86" s="136"/>
+      <c r="H86" s="137"/>
+      <c r="I86" s="138"/>
       <c r="J86" s="13"/>
       <c r="K86" s="13"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A87" s="152" t="s">
+      <c r="A87" s="135" t="s">
         <v>180</v>
       </c>
-      <c r="B87" s="152"/>
-      <c r="C87" s="152"/>
+      <c r="B87" s="135"/>
+      <c r="C87" s="135"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
       <c r="F87" s="14"/>
-      <c r="G87" s="135"/>
-      <c r="H87" s="164"/>
-      <c r="I87" s="136"/>
+      <c r="G87" s="136"/>
+      <c r="H87" s="137"/>
+      <c r="I87" s="138"/>
       <c r="J87" s="13"/>
       <c r="K87" s="13"/>
     </row>
@@ -7602,48 +7602,203 @@
       <c r="F88" s="14"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A89" s="157" t="s">
+      <c r="A89" s="139" t="s">
         <v>181</v>
       </c>
-      <c r="B89" s="157"/>
-      <c r="C89" s="157"/>
-      <c r="D89" s="157"/>
-      <c r="E89" s="157"/>
-      <c r="F89" s="157"/>
-      <c r="G89" s="157"/>
-      <c r="H89" s="157"/>
-      <c r="I89" s="157"/>
-      <c r="J89" s="157"/>
-      <c r="K89" s="157"/>
+      <c r="B89" s="139"/>
+      <c r="C89" s="139"/>
+      <c r="D89" s="139"/>
+      <c r="E89" s="139"/>
+      <c r="F89" s="139"/>
+      <c r="G89" s="139"/>
+      <c r="H89" s="139"/>
+      <c r="I89" s="139"/>
+      <c r="J89" s="139"/>
+      <c r="K89" s="139"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A90" s="145"/>
-      <c r="B90" s="145"/>
-      <c r="C90" s="145"/>
-      <c r="D90" s="145"/>
-      <c r="E90" s="145"/>
-      <c r="F90" s="145"/>
-      <c r="G90" s="145"/>
-      <c r="H90" s="145"/>
-      <c r="I90" s="145"/>
-      <c r="J90" s="145"/>
-      <c r="K90" s="145"/>
+      <c r="A90" s="134"/>
+      <c r="B90" s="134"/>
+      <c r="C90" s="134"/>
+      <c r="D90" s="134"/>
+      <c r="E90" s="134"/>
+      <c r="F90" s="134"/>
+      <c r="G90" s="134"/>
+      <c r="H90" s="134"/>
+      <c r="I90" s="134"/>
+      <c r="J90" s="134"/>
+      <c r="K90" s="134"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A91" s="145"/>
-      <c r="B91" s="145"/>
-      <c r="C91" s="145"/>
-      <c r="D91" s="145"/>
-      <c r="E91" s="145"/>
-      <c r="F91" s="145"/>
-      <c r="G91" s="145"/>
-      <c r="H91" s="145"/>
-      <c r="I91" s="145"/>
-      <c r="J91" s="145"/>
-      <c r="K91" s="145"/>
+      <c r="A91" s="134"/>
+      <c r="B91" s="134"/>
+      <c r="C91" s="134"/>
+      <c r="D91" s="134"/>
+      <c r="E91" s="134"/>
+      <c r="F91" s="134"/>
+      <c r="G91" s="134"/>
+      <c r="H91" s="134"/>
+      <c r="I91" s="134"/>
+      <c r="J91" s="134"/>
+      <c r="K91" s="134"/>
     </row>
   </sheetData>
   <mergeCells count="168">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="G42:K42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="G55:I55"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="G56:I56"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="G57:I57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="G58:I58"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="G69:I69"/>
+    <mergeCell ref="G63:I63"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="G66:I66"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="G75:K75"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="G76:I76"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="G70:I70"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="G71:I71"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="G80:I80"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="G81:I81"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="G82:I82"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="G77:I77"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="G78:I78"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="G79:I79"/>
     <mergeCell ref="A91:K91"/>
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="G86:I86"/>
@@ -7657,161 +7812,6 @@
     <mergeCell ref="G84:I84"/>
     <mergeCell ref="A85:C85"/>
     <mergeCell ref="G85:I85"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="G80:I80"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="G81:I81"/>
-    <mergeCell ref="A82:C82"/>
-    <mergeCell ref="G82:I82"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="G77:I77"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="G78:I78"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="G79:I79"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="G74:I74"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="G75:K75"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="G76:I76"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="G70:I70"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="G71:I71"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="G73:I73"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="G69:I69"/>
-    <mergeCell ref="G63:I63"/>
-    <mergeCell ref="A64:E64"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="G66:I66"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="G61:I61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="G57:I57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="G58:I58"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="G59:I59"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="G55:I55"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="G56:I56"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="G42:K42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="G10:K10"/>
   </mergeCells>
   <pageMargins left="0.5" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7835,205 +7835,205 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="160" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="178" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="168"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="176" t="s">
+      <c r="B2" s="179"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="187" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="177" t="s">
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="187"/>
+      <c r="M2" s="188" t="s">
         <v>184</v>
       </c>
-      <c r="N2" s="178"/>
-      <c r="O2" s="181"/>
-      <c r="P2" s="181"/>
-      <c r="Q2" s="182"/>
+      <c r="N2" s="189"/>
+      <c r="O2" s="192"/>
+      <c r="P2" s="192"/>
+      <c r="Q2" s="193"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="170"/>
-      <c r="B3" s="171"/>
-      <c r="C3" s="172"/>
-      <c r="D3" s="176" t="s">
+      <c r="A3" s="181"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="187" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="179"/>
-      <c r="N3" s="180"/>
-      <c r="O3" s="162"/>
-      <c r="P3" s="162"/>
-      <c r="Q3" s="163"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="187"/>
+      <c r="M3" s="190"/>
+      <c r="N3" s="191"/>
+      <c r="O3" s="145"/>
+      <c r="P3" s="145"/>
+      <c r="Q3" s="146"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="170"/>
-      <c r="B4" s="171"/>
-      <c r="C4" s="172"/>
-      <c r="D4" s="176" t="s">
+      <c r="A4" s="181"/>
+      <c r="B4" s="182"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="187" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="176"/>
-      <c r="J4" s="176"/>
-      <c r="K4" s="176"/>
-      <c r="L4" s="176"/>
-      <c r="M4" s="177" t="s">
+      <c r="E4" s="187"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="187"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="187"/>
+      <c r="M4" s="188" t="s">
         <v>44</v>
       </c>
-      <c r="N4" s="178"/>
-      <c r="O4" s="181"/>
-      <c r="P4" s="181"/>
-      <c r="Q4" s="182"/>
+      <c r="N4" s="189"/>
+      <c r="O4" s="192"/>
+      <c r="P4" s="192"/>
+      <c r="Q4" s="193"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
-      <c r="C5" s="175"/>
-      <c r="D5" s="176" t="s">
+      <c r="A5" s="184"/>
+      <c r="B5" s="185"/>
+      <c r="C5" s="186"/>
+      <c r="D5" s="187" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="176"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="176"/>
-      <c r="H5" s="176"/>
-      <c r="I5" s="176"/>
-      <c r="J5" s="176"/>
-      <c r="K5" s="176"/>
-      <c r="L5" s="176"/>
-      <c r="M5" s="179"/>
-      <c r="N5" s="180"/>
-      <c r="O5" s="162"/>
-      <c r="P5" s="162"/>
-      <c r="Q5" s="163"/>
+      <c r="E5" s="187"/>
+      <c r="F5" s="187"/>
+      <c r="G5" s="187"/>
+      <c r="H5" s="187"/>
+      <c r="I5" s="187"/>
+      <c r="J5" s="187"/>
+      <c r="K5" s="187"/>
+      <c r="L5" s="187"/>
+      <c r="M5" s="190"/>
+      <c r="N5" s="191"/>
+      <c r="O5" s="145"/>
+      <c r="P5" s="145"/>
+      <c r="Q5" s="146"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="165" t="s">
+      <c r="A6" s="171" t="s">
         <v>185</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C6" s="189" t="s">
+      <c r="C6" s="165" t="s">
         <v>187</v>
       </c>
-      <c r="D6" s="190"/>
-      <c r="E6" s="191"/>
-      <c r="F6" s="192" t="s">
+      <c r="D6" s="166"/>
+      <c r="E6" s="167"/>
+      <c r="F6" s="168" t="s">
         <v>188</v>
       </c>
-      <c r="G6" s="192"/>
-      <c r="H6" s="189" t="s">
+      <c r="G6" s="168"/>
+      <c r="H6" s="165" t="s">
         <v>189</v>
       </c>
-      <c r="I6" s="193"/>
-      <c r="J6" s="193"/>
-      <c r="K6" s="193"/>
-      <c r="L6" s="193"/>
-      <c r="M6" s="193"/>
-      <c r="N6" s="193"/>
-      <c r="O6" s="193"/>
-      <c r="P6" s="193"/>
-      <c r="Q6" s="193"/>
+      <c r="I6" s="169"/>
+      <c r="J6" s="169"/>
+      <c r="K6" s="169"/>
+      <c r="L6" s="169"/>
+      <c r="M6" s="169"/>
+      <c r="N6" s="169"/>
+      <c r="O6" s="169"/>
+      <c r="P6" s="169"/>
+      <c r="Q6" s="169"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="165"/>
-      <c r="B7" s="184" t="s">
+      <c r="A7" s="171"/>
+      <c r="B7" s="170" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="148" t="s">
+      <c r="C7" s="158" t="s">
         <v>191</v>
       </c>
-      <c r="D7" s="187" t="s">
+      <c r="D7" s="172" t="s">
         <v>192</v>
       </c>
-      <c r="E7" s="188" t="s">
+      <c r="E7" s="173" t="s">
         <v>193</v>
       </c>
-      <c r="F7" s="183" t="s">
+      <c r="F7" s="174" t="s">
         <v>194</v>
       </c>
-      <c r="G7" s="184" t="s">
+      <c r="G7" s="170" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="185" t="s">
+      <c r="H7" s="175" t="s">
         <v>195</v>
       </c>
-      <c r="I7" s="186"/>
-      <c r="J7" s="186"/>
-      <c r="K7" s="186"/>
-      <c r="L7" s="186"/>
-      <c r="M7" s="186"/>
-      <c r="N7" s="186"/>
-      <c r="O7" s="186"/>
-      <c r="P7" s="186"/>
-      <c r="Q7" s="186"/>
+      <c r="I7" s="176"/>
+      <c r="J7" s="176"/>
+      <c r="K7" s="176"/>
+      <c r="L7" s="176"/>
+      <c r="M7" s="176"/>
+      <c r="N7" s="176"/>
+      <c r="O7" s="176"/>
+      <c r="P7" s="176"/>
+      <c r="Q7" s="176"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="165"/>
-      <c r="B8" s="184"/>
-      <c r="C8" s="148"/>
-      <c r="D8" s="187"/>
-      <c r="E8" s="188"/>
-      <c r="F8" s="183"/>
-      <c r="G8" s="184"/>
-      <c r="H8" s="185"/>
-      <c r="I8" s="186"/>
-      <c r="J8" s="186"/>
-      <c r="K8" s="186"/>
-      <c r="L8" s="186"/>
-      <c r="M8" s="186"/>
-      <c r="N8" s="186"/>
-      <c r="O8" s="186"/>
-      <c r="P8" s="186"/>
-      <c r="Q8" s="186"/>
+      <c r="A8" s="171"/>
+      <c r="B8" s="170"/>
+      <c r="C8" s="158"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="173"/>
+      <c r="F8" s="174"/>
+      <c r="G8" s="170"/>
+      <c r="H8" s="175"/>
+      <c r="I8" s="176"/>
+      <c r="J8" s="176"/>
+      <c r="K8" s="176"/>
+      <c r="L8" s="176"/>
+      <c r="M8" s="176"/>
+      <c r="N8" s="176"/>
+      <c r="O8" s="176"/>
+      <c r="P8" s="176"/>
+      <c r="Q8" s="176"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="165"/>
-      <c r="B9" s="184"/>
-      <c r="C9" s="148"/>
-      <c r="D9" s="187"/>
-      <c r="E9" s="188"/>
-      <c r="F9" s="183"/>
-      <c r="G9" s="184"/>
+      <c r="A9" s="171"/>
+      <c r="B9" s="170"/>
+      <c r="C9" s="158"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="173"/>
+      <c r="F9" s="174"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="17">
         <v>1</v>
       </c>
@@ -8866,94 +8866,94 @@
       <c r="Q51" s="13"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A52" s="165" t="s">
+      <c r="A52" s="171" t="s">
         <v>185</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C52" s="189" t="s">
+      <c r="C52" s="165" t="s">
         <v>187</v>
       </c>
-      <c r="D52" s="193"/>
-      <c r="E52" s="191"/>
-      <c r="F52" s="192" t="s">
+      <c r="D52" s="169"/>
+      <c r="E52" s="167"/>
+      <c r="F52" s="168" t="s">
         <v>188</v>
       </c>
-      <c r="G52" s="192"/>
-      <c r="H52" s="189" t="s">
+      <c r="G52" s="168"/>
+      <c r="H52" s="165" t="s">
         <v>189</v>
       </c>
-      <c r="I52" s="193"/>
-      <c r="J52" s="193"/>
-      <c r="K52" s="193"/>
-      <c r="L52" s="193"/>
-      <c r="M52" s="193"/>
-      <c r="N52" s="193"/>
-      <c r="O52" s="193"/>
-      <c r="P52" s="193"/>
-      <c r="Q52" s="193"/>
+      <c r="I52" s="169"/>
+      <c r="J52" s="169"/>
+      <c r="K52" s="169"/>
+      <c r="L52" s="169"/>
+      <c r="M52" s="169"/>
+      <c r="N52" s="169"/>
+      <c r="O52" s="169"/>
+      <c r="P52" s="169"/>
+      <c r="Q52" s="169"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A53" s="165"/>
-      <c r="B53" s="184" t="s">
+      <c r="A53" s="171"/>
+      <c r="B53" s="170" t="s">
         <v>190</v>
       </c>
-      <c r="C53" s="148" t="s">
+      <c r="C53" s="158" t="s">
         <v>191</v>
       </c>
-      <c r="D53" s="187" t="s">
+      <c r="D53" s="172" t="s">
         <v>192</v>
       </c>
-      <c r="E53" s="188" t="s">
+      <c r="E53" s="173" t="s">
         <v>193</v>
       </c>
-      <c r="F53" s="183" t="s">
+      <c r="F53" s="174" t="s">
         <v>194</v>
       </c>
-      <c r="G53" s="184" t="s">
+      <c r="G53" s="170" t="s">
         <v>50</v>
       </c>
-      <c r="H53" s="185" t="s">
+      <c r="H53" s="175" t="s">
         <v>195</v>
       </c>
-      <c r="I53" s="186"/>
-      <c r="J53" s="186"/>
-      <c r="K53" s="186"/>
-      <c r="L53" s="186"/>
-      <c r="M53" s="186"/>
-      <c r="N53" s="186"/>
-      <c r="O53" s="186"/>
-      <c r="P53" s="186"/>
-      <c r="Q53" s="186"/>
+      <c r="I53" s="176"/>
+      <c r="J53" s="176"/>
+      <c r="K53" s="176"/>
+      <c r="L53" s="176"/>
+      <c r="M53" s="176"/>
+      <c r="N53" s="176"/>
+      <c r="O53" s="176"/>
+      <c r="P53" s="176"/>
+      <c r="Q53" s="176"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A54" s="165"/>
-      <c r="B54" s="184"/>
-      <c r="C54" s="148"/>
-      <c r="D54" s="187"/>
-      <c r="E54" s="188"/>
-      <c r="F54" s="183"/>
-      <c r="G54" s="184"/>
-      <c r="H54" s="185"/>
-      <c r="I54" s="186"/>
-      <c r="J54" s="186"/>
-      <c r="K54" s="186"/>
-      <c r="L54" s="186"/>
-      <c r="M54" s="186"/>
-      <c r="N54" s="186"/>
-      <c r="O54" s="186"/>
-      <c r="P54" s="186"/>
-      <c r="Q54" s="186"/>
+      <c r="A54" s="171"/>
+      <c r="B54" s="170"/>
+      <c r="C54" s="158"/>
+      <c r="D54" s="172"/>
+      <c r="E54" s="173"/>
+      <c r="F54" s="174"/>
+      <c r="G54" s="170"/>
+      <c r="H54" s="175"/>
+      <c r="I54" s="176"/>
+      <c r="J54" s="176"/>
+      <c r="K54" s="176"/>
+      <c r="L54" s="176"/>
+      <c r="M54" s="176"/>
+      <c r="N54" s="176"/>
+      <c r="O54" s="176"/>
+      <c r="P54" s="176"/>
+      <c r="Q54" s="176"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A55" s="165"/>
-      <c r="B55" s="184"/>
-      <c r="C55" s="148"/>
-      <c r="D55" s="187"/>
-      <c r="E55" s="188"/>
-      <c r="F55" s="183"/>
-      <c r="G55" s="184"/>
+      <c r="A55" s="171"/>
+      <c r="B55" s="170"/>
+      <c r="C55" s="158"/>
+      <c r="D55" s="172"/>
+      <c r="E55" s="173"/>
+      <c r="F55" s="174"/>
+      <c r="G55" s="170"/>
       <c r="H55" s="17">
         <v>1</v>
       </c>
@@ -9824,66 +9824,85 @@
       <c r="Q99" s="13"/>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A101" s="157" t="s">
+      <c r="A101" s="139" t="s">
         <v>181</v>
       </c>
-      <c r="B101" s="157"/>
-      <c r="C101" s="157"/>
-      <c r="D101" s="157"/>
-      <c r="E101" s="157"/>
-      <c r="F101" s="157"/>
-      <c r="G101" s="157"/>
-      <c r="H101" s="157"/>
-      <c r="I101" s="157"/>
-      <c r="J101" s="157"/>
-      <c r="K101" s="157"/>
-      <c r="L101" s="157"/>
-      <c r="M101" s="157"/>
-      <c r="N101" s="157"/>
-      <c r="O101" s="157"/>
-      <c r="P101" s="157"/>
-      <c r="Q101" s="157"/>
+      <c r="B101" s="139"/>
+      <c r="C101" s="139"/>
+      <c r="D101" s="139"/>
+      <c r="E101" s="139"/>
+      <c r="F101" s="139"/>
+      <c r="G101" s="139"/>
+      <c r="H101" s="139"/>
+      <c r="I101" s="139"/>
+      <c r="J101" s="139"/>
+      <c r="K101" s="139"/>
+      <c r="L101" s="139"/>
+      <c r="M101" s="139"/>
+      <c r="N101" s="139"/>
+      <c r="O101" s="139"/>
+      <c r="P101" s="139"/>
+      <c r="Q101" s="139"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A102" s="162"/>
-      <c r="B102" s="162"/>
-      <c r="C102" s="162"/>
-      <c r="D102" s="162"/>
-      <c r="E102" s="162"/>
-      <c r="F102" s="162"/>
-      <c r="G102" s="162"/>
-      <c r="H102" s="162"/>
-      <c r="I102" s="162"/>
-      <c r="J102" s="162"/>
-      <c r="K102" s="162"/>
-      <c r="L102" s="162"/>
-      <c r="M102" s="162"/>
-      <c r="N102" s="162"/>
-      <c r="O102" s="162"/>
-      <c r="P102" s="162"/>
-      <c r="Q102" s="162"/>
+      <c r="A102" s="145"/>
+      <c r="B102" s="145"/>
+      <c r="C102" s="145"/>
+      <c r="D102" s="145"/>
+      <c r="E102" s="145"/>
+      <c r="F102" s="145"/>
+      <c r="G102" s="145"/>
+      <c r="H102" s="145"/>
+      <c r="I102" s="145"/>
+      <c r="J102" s="145"/>
+      <c r="K102" s="145"/>
+      <c r="L102" s="145"/>
+      <c r="M102" s="145"/>
+      <c r="N102" s="145"/>
+      <c r="O102" s="145"/>
+      <c r="P102" s="145"/>
+      <c r="Q102" s="145"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A103" s="164"/>
-      <c r="B103" s="164"/>
-      <c r="C103" s="164"/>
-      <c r="D103" s="164"/>
-      <c r="E103" s="164"/>
-      <c r="F103" s="164"/>
-      <c r="G103" s="164"/>
-      <c r="H103" s="164"/>
-      <c r="I103" s="164"/>
-      <c r="J103" s="164"/>
-      <c r="K103" s="164"/>
-      <c r="L103" s="164"/>
-      <c r="M103" s="164"/>
-      <c r="N103" s="164"/>
-      <c r="O103" s="164"/>
-      <c r="P103" s="164"/>
-      <c r="Q103" s="164"/>
+      <c r="A103" s="137"/>
+      <c r="B103" s="137"/>
+      <c r="C103" s="137"/>
+      <c r="D103" s="137"/>
+      <c r="E103" s="137"/>
+      <c r="F103" s="137"/>
+      <c r="G103" s="137"/>
+      <c r="H103" s="137"/>
+      <c r="I103" s="137"/>
+      <c r="J103" s="137"/>
+      <c r="K103" s="137"/>
+      <c r="L103" s="137"/>
+      <c r="M103" s="137"/>
+      <c r="N103" s="137"/>
+      <c r="O103" s="137"/>
+      <c r="P103" s="137"/>
+      <c r="Q103" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:C5"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="M2:N3"/>
+    <mergeCell ref="O2:Q3"/>
+    <mergeCell ref="D3:L3"/>
+    <mergeCell ref="D4:L4"/>
+    <mergeCell ref="M4:N5"/>
+    <mergeCell ref="O4:Q5"/>
+    <mergeCell ref="D5:L5"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="G53:G55"/>
+    <mergeCell ref="H53:Q54"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H7:Q8"/>
     <mergeCell ref="A101:Q101"/>
     <mergeCell ref="A102:Q102"/>
     <mergeCell ref="A103:Q103"/>
@@ -9900,25 +9919,6 @@
     <mergeCell ref="C53:C55"/>
     <mergeCell ref="D53:D55"/>
     <mergeCell ref="E53:E55"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="G53:G55"/>
-    <mergeCell ref="H53:Q54"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H7:Q8"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:C5"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="M2:N3"/>
-    <mergeCell ref="O2:Q3"/>
-    <mergeCell ref="D3:L3"/>
-    <mergeCell ref="D4:L4"/>
-    <mergeCell ref="M4:N5"/>
-    <mergeCell ref="O4:Q5"/>
-    <mergeCell ref="D5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11710,8 +11710,8 @@
   </sheetPr>
   <dimension ref="A1:N657"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A565" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A505" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A511" sqref="A511:A522"/>
     </sheetView>
   </sheetViews>
@@ -36131,9 +36131,9 @@
   </sheetPr>
   <dimension ref="A1:BM111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42469,7 +42469,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BL111" xr:uid="{FED45917-8414-4A4C-A61B-1109AAA4B730}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BL112">
     <sortCondition ref="B2:B112"/>
     <sortCondition ref="C2:C112"/>
@@ -42482,4 +42481,278 @@
   <pageMargins left="0.5" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="28" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010077DB800C29E38A4082BE3FE3AD5BB76A" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="57bfd154d00f9d412063991bd8d7f7ca">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0A814B8E-0CF5-46E4-A9C0-BFEB2CB7B5DC" xmlns:ns3="0a814b8e-0cf5-46e4-a9c0-bfeb2cb7b5dc" xmlns:ns4="84fa792b-db08-4e92-885f-28de3837c9fa" xmlns:ns5="6f98d64a-07ba-4b39-8e6f-dd01000050b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ce92682e6f136e01c8e36811ac4f639" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
+    <xsd:import namespace="0A814B8E-0CF5-46E4-A9C0-BFEB2CB7B5DC"/>
+    <xsd:import namespace="0a814b8e-0cf5-46e4-a9c0-bfeb2cb7b5dc"/>
+    <xsd:import namespace="84fa792b-db08-4e92-885f-28de3837c9fa"/>
+    <xsd:import namespace="6f98d64a-07ba-4b39-8e6f-dd01000050b1"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:Doc_x0020_Category" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns5:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0A814B8E-0CF5-46E4-A9C0-BFEB2CB7B5DC" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Doc_x0020_Category" ma:index="8" nillable="true" ma:displayName="Doc Category" ma:format="Dropdown" ma:internalName="Doc_x0020_Category">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Thermalito Restoration"/>
+          <xsd:enumeration value="SONET Upgrade Project"/>
+          <xsd:enumeration value="DWR-LindaRogersShare"/>
+          <xsd:enumeration value="DWR-LightriverShare"/>
+          <xsd:enumeration value="Help Files"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0a814b8e-0cf5-46e4-a9c0-bfeb2cb7b5dc" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="18" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="651b62a4-9796-44f9-b2a5-9cb121c10878" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="84fa792b-db08-4e92-885f-28de3837c9fa" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6f98d64a-07ba-4b39-8e6f-dd01000050b1" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{A6123CB7-368B-413B-939B-0D92AF1535F3}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="{84fa792b-db08-4e92-885f-28de3837c9fa}">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6B6863A-DBFE-4892-B0D2-CA564DBD3B36}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22B2953D-0E62-43BB-8C3A-E83A36B90269}"/>
 </file>
</xml_diff>